<commit_message>
SC Charge List excel state removed, name changes
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SC-Charges-List-Template.xlsx
+++ b/application/controllers/excel-templates/SC-Charges-List-Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-dev\application\controllers\excel-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-aws\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Jobcard Code</t>
   </si>
   <si>
-    <t>State</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
   </si>
   <si>
     <t>Customer Total Rs.</t>
-  </si>
-  <si>
-    <t>{sc:state}</t>
   </si>
   <si>
     <t>{sc:product}</t>
@@ -427,27 +421,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" customWidth="1"/>
-    <col min="7" max="7" width="42.5703125" customWidth="1"/>
-    <col min="8" max="9" width="33.42578125" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="42.5703125" customWidth="1"/>
+    <col min="7" max="8" width="33.42578125" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,57 +457,51 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upload vendor pincode changes
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SC-Charges-List-Template.xlsx
+++ b/application/controllers/excel-templates/SC-Charges-List-Template.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Jobcard Code</t>
   </si>
   <si>
-    <t>State</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
   </si>
   <si>
     <t>Customer Total Rs.</t>
-  </si>
-  <si>
-    <t>{sc:state}</t>
   </si>
   <si>
     <t>{sc:product}</t>
@@ -427,27 +421,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" customWidth="1"/>
-    <col min="7" max="7" width="42.5703125" customWidth="1"/>
-    <col min="8" max="9" width="33.42578125" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="42.5703125" customWidth="1"/>
+    <col min="7" max="8" width="33.42578125" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,57 +457,51 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SC List view on vendor panel, Downloadable in our CRM
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SC-Charges-List-Template.xlsx
+++ b/application/controllers/excel-templates/SC-Charges-List-Template.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Jobcard Code</t>
   </si>
   <si>
-    <t>State</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
   </si>
   <si>
     <t>Customer Total Rs.</t>
-  </si>
-  <si>
-    <t>{sc:state}</t>
   </si>
   <si>
     <t>{sc:product}</t>
@@ -427,27 +421,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" customWidth="1"/>
-    <col min="7" max="7" width="42.5703125" customWidth="1"/>
-    <col min="8" max="9" width="33.42578125" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="42.5703125" customWidth="1"/>
+    <col min="7" max="8" width="33.42578125" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,57 +457,51 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SC Charges Download Excel Template Changes
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SC-Charges-List-Template.xlsx
+++ b/application/controllers/excel-templates/SC-Charges-List-Template.xlsx
@@ -2,32 +2,32 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-dev\application\controllers\excel-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bredkhan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>Jobcard Code</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Product</t>
   </si>
@@ -38,12 +38,6 @@
     <t>Capacity</t>
   </si>
   <si>
-    <t>Service Category</t>
-  </si>
-  <si>
-    <t>Customer Total Rs.</t>
-  </si>
-  <si>
     <t>{sc:product}</t>
   </si>
   <si>
@@ -65,32 +59,63 @@
     <t>{sc:sc_code}</t>
   </si>
   <si>
-    <t>Vendor Total</t>
-  </si>
-  <si>
     <t>{sc:vendor_total}</t>
   </si>
   <si>
-    <t>Vendor Basic Charge</t>
-  </si>
-  <si>
-    <t>Vendor Tax</t>
-  </si>
-  <si>
-    <t>Serial Number Mandatory</t>
-  </si>
-  <si>
-    <t>{sc:pod}</t>
-  </si>
-  <si>
     <t>{sc:customer_net_payable}</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>{sc:state}</t>
+  </si>
+  <si>
+    <t>1 Month Warranty on Service &amp; Installation</t>
+  </si>
+  <si>
+    <t>3 Months Warranty on Refrigerant Gas Filling</t>
+  </si>
+  <si>
+    <t>247around Royalty 5% On Parts</t>
+  </si>
+  <si>
+    <t>247around Royalty 15% On Extra Repair Charges</t>
+  </si>
+  <si>
+    <t>Jobcard 
+Code</t>
+  </si>
+  <si>
+    <t>Service 
+Category</t>
+  </si>
+  <si>
+    <t>Vendor 
+Basic Charge</t>
+  </si>
+  <si>
+    <t>Vendor 
+Tax</t>
+  </si>
+  <si>
+    <t>Vendor Total 
+With Tax and 
+Incentive (Rs.)</t>
+  </si>
+  <si>
+    <t>Customer 
+Total Rs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                            Indias No.1 Analytics Based Appliance Repair Brand</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,16 +131,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -123,22 +174,205 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -156,6 +390,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>413656</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>67127</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>150560</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>159544</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6538231" y="257627"/>
+          <a:ext cx="613204" cy="673442"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -421,90 +704,216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
-    <col min="6" max="6" width="42.5703125" customWidth="1"/>
-    <col min="7" max="8" width="33.42578125" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="19"/>
+    </row>
+    <row r="10" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D10" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E10" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F10" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D11" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="E11" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="F11" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="G11" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="I11" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>18</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="69" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SC Charges Template Modified
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SC-Charges-List-Template.xlsx
+++ b/application/controllers/excel-templates/SC-Charges-List-Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bredkhan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-dev\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -91,14 +91,6 @@
 Category</t>
   </si>
   <si>
-    <t>Vendor 
-Basic Charge</t>
-  </si>
-  <si>
-    <t>Vendor 
-Tax</t>
-  </si>
-  <si>
     <t>Vendor Total 
 With Tax and 
 Incentive (Rs.)</t>
@@ -109,6 +101,14 @@
   </si>
   <si>
     <t xml:space="preserve">                                                            Indias No.1 Analytics Based Appliance Repair Brand</t>
+  </si>
+  <si>
+    <t>Vendor 
+Basic Charge Rs.</t>
+  </si>
+  <si>
+    <t>Vendor 
+Tax Rs.</t>
   </si>
 </sst>
 </file>
@@ -710,7 +710,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +745,7 @@
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E2" s="16"/>
       <c r="F2" s="15"/>
@@ -866,16 +866,16 @@
         <v>19</v>
       </c>
       <c r="G10" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="J10" s="23" t="s">
         <v>21</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" s="23" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
RM dashboard Header Changes And Remove State From Download Basic Charge For Service Centers
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SC-Charges-List-Template.xlsx
+++ b/application/controllers/excel-templates/SC-Charges-List-Template.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-dev\application\controllers\excel-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Product</t>
   </si>
@@ -63,12 +63,6 @@
   </si>
   <si>
     <t>{sc:customer_net_payable}</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>{sc:state}</t>
   </si>
   <si>
     <t>1 Month Warranty on Service &amp; Installation</t>
@@ -114,7 +108,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -166,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -175,17 +169,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -206,32 +189,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color auto="1"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -255,19 +218,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -295,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -306,31 +256,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -345,34 +289,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -396,20 +331,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>413656</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>67127</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>150560</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>595059</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>159544</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -703,14 +644,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,185 +669,170 @@
     <col min="11" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="5"/>
       <c r="I1" s="6"/>
-      <c r="J1" s="7"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="16"/>
+    </row>
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="12"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="12"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="12"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="12"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="12"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="12"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="19"/>
-    </row>
-    <row r="10" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="21" t="s">
+      <c r="H10" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="21" t="s">
+      <c r="I10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="25" t="s">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="B11" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="C11" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="D11" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="E11" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="F11" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="G11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="H11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="I11" s="21" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>